<commit_message>
aggiornamento excel retail e test XRA_factoring
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Library_Formula" sheetId="2" r:id="rId2"/>
     <sheet name="Formula Libraries Labels" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
   <si>
     <t>Action</t>
   </si>
@@ -164,70 +164,70 @@
     <t>Indicatori Italia Retail</t>
   </si>
   <si>
-    <t>UpdateAnalysisUnit_RETAIL</t>
-  </si>
-  <si>
-    <t>updateOutputTable_RETAIL</t>
-  </si>
-  <si>
     <t>UNION_INDICATORS</t>
   </si>
   <si>
-    <t>IND_2</t>
-  </si>
-  <si>
-    <t>IND_6</t>
-  </si>
-  <si>
-    <t>IND_7</t>
-  </si>
-  <si>
-    <t>IND_10</t>
-  </si>
-  <si>
-    <t>IND_11</t>
-  </si>
-  <si>
-    <t>IND_12</t>
-  </si>
-  <si>
-    <t>IND_13</t>
-  </si>
-  <si>
-    <t>IND_15</t>
-  </si>
-  <si>
-    <t>IND_16</t>
-  </si>
-  <si>
-    <t>IND_17</t>
-  </si>
-  <si>
-    <t>IND_18</t>
-  </si>
-  <si>
-    <t>IND_22</t>
-  </si>
-  <si>
-    <t>IND_26</t>
-  </si>
-  <si>
-    <t>IND_27</t>
-  </si>
-  <si>
-    <t>IND_28</t>
-  </si>
-  <si>
-    <t>IND_29</t>
-  </si>
-  <si>
-    <t>IND_31</t>
-  </si>
-  <si>
-    <t>IND_34</t>
-  </si>
-  <si>
-    <t>IND_35</t>
+    <t>INDICATOR_2</t>
+  </si>
+  <si>
+    <t>INDICATOR_6</t>
+  </si>
+  <si>
+    <t>INDICATOR_7</t>
+  </si>
+  <si>
+    <t>INDICATOR_10</t>
+  </si>
+  <si>
+    <t>INDICATOR_11</t>
+  </si>
+  <si>
+    <t>INDICATOR_12</t>
+  </si>
+  <si>
+    <t>INDICATOR_13</t>
+  </si>
+  <si>
+    <t>INDICATOR_15</t>
+  </si>
+  <si>
+    <t>INDICATOR_16</t>
+  </si>
+  <si>
+    <t>INDICATOR_17</t>
+  </si>
+  <si>
+    <t>INDICATOR_18</t>
+  </si>
+  <si>
+    <t>INDICATOR_22</t>
+  </si>
+  <si>
+    <t>INDICATOR_26</t>
+  </si>
+  <si>
+    <t>INDICATOR_27</t>
+  </si>
+  <si>
+    <t>INDICATOR_28</t>
+  </si>
+  <si>
+    <t>INDICATOR_29</t>
+  </si>
+  <si>
+    <t>INDICATOR_31</t>
+  </si>
+  <si>
+    <t>INDICATOR_34</t>
+  </si>
+  <si>
+    <t>INDICATOR_35</t>
+  </si>
+  <si>
+    <t>UpdateAnalysisUnit_IT</t>
+  </si>
+  <si>
+    <t>updateOutputTable_IT</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -868,11 +868,14 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -899,7 +902,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -916,7 +919,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
@@ -932,8 +935,8 @@
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -950,7 +953,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -967,7 +970,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
@@ -984,7 +987,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
@@ -1001,7 +1004,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
@@ -1018,7 +1021,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
@@ -1035,7 +1038,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -1052,7 +1055,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>13</v>
@@ -1069,7 +1072,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
@@ -1086,7 +1089,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
@@ -1103,7 +1106,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
@@ -1120,7 +1123,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
@@ -1137,7 +1140,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
@@ -1154,7 +1157,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -1171,7 +1174,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
@@ -1188,7 +1191,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>13</v>
@@ -1205,7 +1208,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>13</v>
@@ -1222,7 +1225,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>13</v>
@@ -1239,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
@@ -1292,21 +1295,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1420,30 +1408,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1457,4 +1437,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunti indicatori retail nella union e negli excel delle instance
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\13_LIB_EWS_RETAIL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\13_LIB_EWS_RETAIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="1785" windowWidth="25485" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="4185" yWindow="1785" windowWidth="25485" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
     <sheet name="Library_Formula" sheetId="2" r:id="rId2"/>
     <sheet name="Formula Libraries Labels" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="103">
   <si>
     <t>Action</t>
   </si>
@@ -228,12 +228,201 @@
   </si>
   <si>
     <t>updateOutputTable_IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_52 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_53 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_54 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_55 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_60 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_61 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_62 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_63 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_70 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_71 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_80 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_81 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_82 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_83 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_84 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_85 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_86 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDICATOR_87 </t>
+  </si>
+  <si>
+    <t>INDICATOR_100</t>
+  </si>
+  <si>
+    <t>INDICATOR_114</t>
+  </si>
+  <si>
+    <t>INDICATOR_201</t>
+  </si>
+  <si>
+    <t>INDICATOR_202</t>
+  </si>
+  <si>
+    <t>INDICATOR_203</t>
+  </si>
+  <si>
+    <t>INDICATOR_204</t>
+  </si>
+  <si>
+    <t>INDICATOR_205</t>
+  </si>
+  <si>
+    <t>INDICATOR_206</t>
+  </si>
+  <si>
+    <t>INDICATOR_207</t>
+  </si>
+  <si>
+    <t>INDICATOR_208</t>
+  </si>
+  <si>
+    <t>INDICATOR_209</t>
+  </si>
+  <si>
+    <t>INDICATOR_210</t>
+  </si>
+  <si>
+    <t>INDICATOR_211</t>
+  </si>
+  <si>
+    <t>INDICATOR_212</t>
+  </si>
+  <si>
+    <t>INDICATOR_213</t>
+  </si>
+  <si>
+    <t>INDICATOR_214</t>
+  </si>
+  <si>
+    <t>INDICATOR_215</t>
+  </si>
+  <si>
+    <t>INDICATOR_216</t>
+  </si>
+  <si>
+    <t>INDICATOR_217</t>
+  </si>
+  <si>
+    <t>INDICATOR_218</t>
+  </si>
+  <si>
+    <t>INDICATOR_219</t>
+  </si>
+  <si>
+    <t>INDICATOR_220</t>
+  </si>
+  <si>
+    <t>INDICATOR_221</t>
+  </si>
+  <si>
+    <t>INDICATOR_222</t>
+  </si>
+  <si>
+    <t>INDICATOR_223</t>
+  </si>
+  <si>
+    <t>INDICATOR_224</t>
+  </si>
+  <si>
+    <t>INDICATOR_225</t>
+  </si>
+  <si>
+    <t>INDICATOR_226</t>
+  </si>
+  <si>
+    <t>INDICATOR_227</t>
+  </si>
+  <si>
+    <t>INDICATOR_228</t>
+  </si>
+  <si>
+    <t>INDICATOR_229</t>
+  </si>
+  <si>
+    <t>INDICATOR_230</t>
+  </si>
+  <si>
+    <t>INDICATOR_231</t>
+  </si>
+  <si>
+    <t>INDICATOR_106</t>
+  </si>
+  <si>
+    <t>INDICATOR_107</t>
+  </si>
+  <si>
+    <t>INDICATOR_108</t>
+  </si>
+  <si>
+    <t>INDICATOR_109</t>
+  </si>
+  <si>
+    <t>INDICATOR_110</t>
+  </si>
+  <si>
+    <t>INDICATOR_111</t>
+  </si>
+  <si>
+    <t>INDICATOR_112</t>
+  </si>
+  <si>
+    <t>INDICATOR_113</t>
+  </si>
+  <si>
+    <t>INDICATOR_115</t>
+  </si>
+  <si>
+    <t>INDICATOR_116</t>
+  </si>
+  <si>
+    <t>INDICATOR_117</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -782,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -823,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1248,6 +1437,1077 @@
         <v>13</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1409,18 +2669,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1440,14 +2700,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1460,4 +2712,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunti indicatori in attesa alla union e aggiornate le variable, altri piccoli fix
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="118">
   <si>
     <t>Action</t>
   </si>
@@ -444,6 +444,24 @@
   </si>
   <si>
     <t>INDICATOR_151</t>
+  </si>
+  <si>
+    <t>INDICATOR_101</t>
+  </si>
+  <si>
+    <t>INDICATOR_102</t>
+  </si>
+  <si>
+    <t>INDICATOR_103</t>
+  </si>
+  <si>
+    <t>INDICATOR_105</t>
+  </si>
+  <si>
+    <t>INDICATOR_112</t>
+  </si>
+  <si>
+    <t>INDICATOR_113</t>
   </si>
 </sst>
 </file>
@@ -1063,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C96" sqref="C9:C96"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1975,7 +1993,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>13</v>
@@ -1991,8 +2009,8 @@
       <c r="B54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>109</v>
+      <c r="C54" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>13</v>
@@ -2009,7 +2027,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>13</v>
@@ -2025,8 +2043,8 @@
       <c r="B56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>43</v>
+      <c r="C56" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>13</v>
@@ -2043,7 +2061,7 @@
         <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>13</v>
@@ -2059,8 +2077,8 @@
       <c r="B58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>45</v>
+      <c r="C58" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>13</v>
@@ -2077,7 +2095,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -2094,7 +2112,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>13</v>
@@ -2111,7 +2129,7 @@
         <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>13</v>
@@ -2128,7 +2146,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>13</v>
@@ -2145,7 +2163,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>13</v>
@@ -2162,7 +2180,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>13</v>
@@ -2179,7 +2197,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>13</v>
@@ -2196,7 +2214,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>13</v>
@@ -2213,7 +2231,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>13</v>
@@ -2230,7 +2248,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>13</v>
@@ -2247,7 +2265,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>13</v>
@@ -2264,7 +2282,7 @@
         <v>16</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>13</v>
@@ -2281,7 +2299,7 @@
         <v>16</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>13</v>
@@ -2298,7 +2316,7 @@
         <v>16</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>13</v>
@@ -2315,7 +2333,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>13</v>
@@ -2332,7 +2350,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>13</v>
@@ -2349,7 +2367,7 @@
         <v>16</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>13</v>
@@ -2366,7 +2384,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>13</v>
@@ -2383,7 +2401,7 @@
         <v>16</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>13</v>
@@ -2400,7 +2418,7 @@
         <v>16</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>13</v>
@@ -2417,7 +2435,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>13</v>
@@ -2434,7 +2452,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>13</v>
@@ -2451,7 +2469,7 @@
         <v>16</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>13</v>
@@ -2468,7 +2486,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>13</v>
@@ -2485,7 +2503,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>13</v>
@@ -2502,7 +2520,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>13</v>
@@ -2519,7 +2537,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>13</v>
@@ -2536,7 +2554,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>13</v>
@@ -2553,7 +2571,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>13</v>
@@ -2570,7 +2588,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>13</v>
@@ -2587,7 +2605,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>13</v>
@@ -2604,7 +2622,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>13</v>
@@ -2621,7 +2639,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>13</v>
@@ -2638,7 +2656,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>13</v>
@@ -2655,7 +2673,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>13</v>
@@ -2672,7 +2690,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>13</v>
@@ -2688,8 +2706,8 @@
       <c r="B95" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>110</v>
+      <c r="C95" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>13</v>
@@ -2705,13 +2723,115 @@
       <c r="B96" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="1" t="s">
+      <c r="E102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2759,15 +2879,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2881,6 +2992,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2888,14 +3008,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2907,6 +3019,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Aggiunta pt4 e modificati indicatori e rispettive formule
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="119">
   <si>
     <t>Action</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>INDICATOR_113</t>
+  </si>
+  <si>
+    <t>UNION_INDICATORS_PT4</t>
   </si>
 </sst>
 </file>
@@ -1081,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1228,7 +1231,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
@@ -1245,7 +1248,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
@@ -1261,8 +1264,8 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
@@ -1279,7 +1282,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
@@ -1296,7 +1299,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -1313,7 +1316,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>13</v>
@@ -1330,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
@@ -1347,7 +1350,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
@@ -1363,8 +1366,8 @@
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>104</v>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
@@ -1381,7 +1384,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
@@ -1397,8 +1400,8 @@
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>27</v>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
@@ -1415,7 +1418,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -1432,7 +1435,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
@@ -1448,8 +1451,8 @@
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>105</v>
+      <c r="C21" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>13</v>
@@ -1466,7 +1469,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>13</v>
@@ -1482,8 +1485,8 @@
       <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>30</v>
+      <c r="C23" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>13</v>
@@ -1500,7 +1503,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
@@ -1517,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
@@ -1534,7 +1537,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>13</v>
@@ -1551,7 +1554,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
@@ -1568,7 +1571,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>13</v>
@@ -1585,7 +1588,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
@@ -1602,7 +1605,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>13</v>
@@ -1618,8 +1621,8 @@
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>107</v>
+      <c r="C31" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>13</v>
@@ -1636,7 +1639,7 @@
         <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>13</v>
@@ -1652,8 +1655,8 @@
       <c r="B33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>84</v>
+      <c r="C33" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>13</v>
@@ -1670,7 +1673,7 @@
         <v>16</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>13</v>
@@ -1687,7 +1690,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>13</v>
@@ -1704,7 +1707,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>13</v>
@@ -1721,7 +1724,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>13</v>
@@ -1738,7 +1741,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>13</v>
@@ -1755,7 +1758,7 @@
         <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>13</v>
@@ -1772,7 +1775,7 @@
         <v>16</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>13</v>
@@ -1789,7 +1792,7 @@
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>13</v>
@@ -1806,7 +1809,7 @@
         <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>13</v>
@@ -1822,8 +1825,8 @@
       <c r="B43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>94</v>
+      <c r="C43" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>13</v>
@@ -1839,8 +1842,8 @@
       <c r="B44" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>95</v>
+      <c r="C44" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>13</v>
@@ -1857,7 +1860,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>13</v>
@@ -1874,7 +1877,7 @@
         <v>16</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>13</v>
@@ -1891,7 +1894,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>13</v>
@@ -1908,7 +1911,7 @@
         <v>16</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>13</v>
@@ -1925,7 +1928,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>13</v>
@@ -1942,7 +1945,7 @@
         <v>16</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>13</v>
@@ -1959,7 +1962,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>13</v>
@@ -1976,7 +1979,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>13</v>
@@ -1993,7 +1996,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>13</v>
@@ -2010,7 +2013,7 @@
         <v>16</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>13</v>
@@ -2027,7 +2030,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>13</v>
@@ -2043,8 +2046,8 @@
       <c r="B56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>115</v>
+      <c r="C56" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>13</v>
@@ -2060,8 +2063,8 @@
       <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>41</v>
+      <c r="C57" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>13</v>
@@ -2077,8 +2080,8 @@
       <c r="B58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>109</v>
+      <c r="C58" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>13</v>
@@ -2094,8 +2097,8 @@
       <c r="B59" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>42</v>
+      <c r="C59" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -2112,7 +2115,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>13</v>
@@ -2129,7 +2132,7 @@
         <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>13</v>
@@ -2146,7 +2149,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>13</v>
@@ -2163,7 +2166,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>13</v>
@@ -2180,7 +2183,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>13</v>
@@ -2197,7 +2200,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>13</v>
@@ -2214,7 +2217,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>13</v>
@@ -2231,7 +2234,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>13</v>
@@ -2248,7 +2251,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>13</v>
@@ -2265,7 +2268,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>13</v>
@@ -2282,7 +2285,7 @@
         <v>16</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>13</v>
@@ -2299,7 +2302,7 @@
         <v>16</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>13</v>
@@ -2316,7 +2319,7 @@
         <v>16</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>13</v>
@@ -2333,7 +2336,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>13</v>
@@ -2350,7 +2353,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>13</v>
@@ -2367,7 +2370,7 @@
         <v>16</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>13</v>
@@ -2384,7 +2387,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>13</v>
@@ -2401,7 +2404,7 @@
         <v>16</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>13</v>
@@ -2418,7 +2421,7 @@
         <v>16</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>13</v>
@@ -2435,7 +2438,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>13</v>
@@ -2452,7 +2455,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>13</v>
@@ -2469,7 +2472,7 @@
         <v>16</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>13</v>
@@ -2486,7 +2489,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>13</v>
@@ -2503,7 +2506,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>13</v>
@@ -2520,7 +2523,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>13</v>
@@ -2537,7 +2540,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>13</v>
@@ -2554,7 +2557,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>13</v>
@@ -2571,7 +2574,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>13</v>
@@ -2588,7 +2591,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>13</v>
@@ -2605,7 +2608,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>13</v>
@@ -2622,7 +2625,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>13</v>
@@ -2639,7 +2642,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>13</v>
@@ -2656,7 +2659,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>13</v>
@@ -2673,7 +2676,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>13</v>
@@ -2690,7 +2693,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>13</v>
@@ -2707,7 +2710,7 @@
         <v>16</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>13</v>
@@ -2724,7 +2727,7 @@
         <v>16</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>13</v>
@@ -2740,8 +2743,8 @@
       <c r="B97" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>117</v>
+      <c r="C97" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>13</v>
@@ -2757,8 +2760,8 @@
       <c r="B98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>79</v>
+      <c r="C98" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>13</v>
@@ -2775,7 +2778,7 @@
         <v>16</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>13</v>
@@ -2792,7 +2795,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>13</v>
@@ -2808,8 +2811,8 @@
       <c r="B101" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>110</v>
+      <c r="C101" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>13</v>
@@ -2826,12 +2829,29 @@
         <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F102" s="1" t="s">
+      <c r="E103" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F103" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2879,6 +2899,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2992,22 +3027,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3021,27 +3064,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add new formula getmodules
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/13_LIB_EWS_RETAIL/13_LibFormula.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\13_LIB_EWS_RETAIL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\13_LIB_EWS_RETAIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="122">
   <si>
     <t>Action</t>
   </si>
@@ -471,12 +471,15 @@
   </si>
   <si>
     <t>INDICATOR_900</t>
+  </si>
+  <si>
+    <t>getAllModulesElaboration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -588,7 +591,7 @@
         <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -637,7 +640,7 @@
         <xdr:cNvPr id="2" name="AutoShape 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -696,7 +699,7 @@
         <xdr:cNvPr id="2052" name="_xssf_cell_comment" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -745,7 +748,7 @@
         <xdr:cNvPr id="2" name="AutoShape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1090,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1168,8 +1171,8 @@
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>39</v>
+      <c r="C4" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -1186,7 +1189,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
@@ -1203,7 +1206,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1220,7 +1223,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -1237,7 +1240,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
@@ -1254,7 +1257,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
@@ -1271,7 +1274,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
@@ -1287,8 +1290,8 @@
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
@@ -1305,7 +1308,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -1322,7 +1325,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>13</v>
@@ -1339,7 +1342,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
@@ -1356,7 +1359,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
@@ -1373,7 +1376,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
@@ -1389,8 +1392,8 @@
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>104</v>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
@@ -1407,7 +1410,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
@@ -1423,8 +1426,8 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>27</v>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
@@ -1441,7 +1444,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
@@ -1458,7 +1461,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>13</v>
@@ -1474,8 +1477,8 @@
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>105</v>
+      <c r="C22" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>13</v>
@@ -1492,7 +1495,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>13</v>
@@ -1508,8 +1511,8 @@
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>30</v>
+      <c r="C24" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
@@ -1526,7 +1529,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
@@ -1543,7 +1546,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>13</v>
@@ -1560,7 +1563,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
@@ -1577,7 +1580,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>13</v>
@@ -1594,7 +1597,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
@@ -1611,7 +1614,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>13</v>
@@ -1628,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>13</v>
@@ -1644,8 +1647,8 @@
       <c r="B32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>107</v>
+      <c r="C32" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>13</v>
@@ -1662,7 +1665,7 @@
         <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>13</v>
@@ -1678,8 +1681,8 @@
       <c r="B34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>84</v>
+      <c r="C34" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>13</v>
@@ -1696,7 +1699,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>13</v>
@@ -1713,7 +1716,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>13</v>
@@ -1730,7 +1733,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>13</v>
@@ -1747,7 +1750,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>13</v>
@@ -1764,7 +1767,7 @@
         <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>13</v>
@@ -1781,7 +1784,7 @@
         <v>16</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>13</v>
@@ -1798,7 +1801,7 @@
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>13</v>
@@ -1815,7 +1818,7 @@
         <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>13</v>
@@ -1832,7 +1835,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>13</v>
@@ -1848,8 +1851,8 @@
       <c r="B44" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>94</v>
+      <c r="C44" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>13</v>
@@ -1865,8 +1868,8 @@
       <c r="B45" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>95</v>
+      <c r="C45" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>13</v>
@@ -1883,7 +1886,7 @@
         <v>16</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>13</v>
@@ -1900,7 +1903,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>13</v>
@@ -1917,7 +1920,7 @@
         <v>16</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>13</v>
@@ -1934,7 +1937,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>13</v>
@@ -1951,7 +1954,7 @@
         <v>16</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>13</v>
@@ -1968,7 +1971,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>13</v>
@@ -1985,7 +1988,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>13</v>
@@ -2002,7 +2005,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>13</v>
@@ -2019,7 +2022,7 @@
         <v>16</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>13</v>
@@ -2036,7 +2039,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>13</v>
@@ -2053,7 +2056,7 @@
         <v>16</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>13</v>
@@ -2069,8 +2072,8 @@
       <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>115</v>
+      <c r="C57" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>13</v>
@@ -2086,8 +2089,8 @@
       <c r="B58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>41</v>
+      <c r="C58" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>13</v>
@@ -2103,8 +2106,8 @@
       <c r="B59" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>109</v>
+      <c r="C59" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -2120,8 +2123,8 @@
       <c r="B60" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>42</v>
+      <c r="C60" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>13</v>
@@ -2138,7 +2141,7 @@
         <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>13</v>
@@ -2155,7 +2158,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>13</v>
@@ -2172,7 +2175,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>13</v>
@@ -2189,7 +2192,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>13</v>
@@ -2206,7 +2209,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>13</v>
@@ -2223,7 +2226,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>13</v>
@@ -2240,7 +2243,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>13</v>
@@ -2257,7 +2260,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>13</v>
@@ -2274,7 +2277,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>13</v>
@@ -2291,7 +2294,7 @@
         <v>16</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>13</v>
@@ -2308,7 +2311,7 @@
         <v>16</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>13</v>
@@ -2325,7 +2328,7 @@
         <v>16</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>13</v>
@@ -2342,7 +2345,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>13</v>
@@ -2359,7 +2362,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>13</v>
@@ -2376,7 +2379,7 @@
         <v>16</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>13</v>
@@ -2393,7 +2396,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>13</v>
@@ -2410,7 +2413,7 @@
         <v>16</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>13</v>
@@ -2427,7 +2430,7 @@
         <v>16</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>13</v>
@@ -2444,7 +2447,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>13</v>
@@ -2461,7 +2464,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>13</v>
@@ -2478,7 +2481,7 @@
         <v>16</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>13</v>
@@ -2495,7 +2498,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>13</v>
@@ -2512,7 +2515,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>13</v>
@@ -2529,7 +2532,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>13</v>
@@ -2546,7 +2549,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>13</v>
@@ -2563,7 +2566,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>13</v>
@@ -2580,7 +2583,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>13</v>
@@ -2597,7 +2600,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>13</v>
@@ -2614,7 +2617,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>13</v>
@@ -2631,7 +2634,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>13</v>
@@ -2648,7 +2651,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>13</v>
@@ -2665,7 +2668,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>13</v>
@@ -2682,7 +2685,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>13</v>
@@ -2699,7 +2702,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>13</v>
@@ -2716,7 +2719,7 @@
         <v>16</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>13</v>
@@ -2733,7 +2736,7 @@
         <v>16</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>13</v>
@@ -2750,7 +2753,7 @@
         <v>16</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>13</v>
@@ -2766,8 +2769,8 @@
       <c r="B98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>117</v>
+      <c r="C98" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>13</v>
@@ -2783,8 +2786,8 @@
       <c r="B99" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>79</v>
+      <c r="C99" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>13</v>
@@ -2801,7 +2804,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>13</v>
@@ -2818,7 +2821,7 @@
         <v>16</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>13</v>
@@ -2834,8 +2837,8 @@
       <c r="B102" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>110</v>
+      <c r="C102" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>13</v>
@@ -2852,7 +2855,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>13</v>
@@ -2869,7 +2872,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>13</v>
@@ -2886,12 +2889,29 @@
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="1" t="s">
+      <c r="E106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2939,6 +2959,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -3052,22 +3087,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3081,27 +3124,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>